<commit_message>
failed effort to add labels from CARINMappingSpreadsheet
</commit_message>
<xml_diff>
--- a/fsh/ig-data/input/images/CARINMappingtoFHIRinterim20200818.xlsx
+++ b/fsh/ig-data/input/images/CARINMappingtoFHIRinterim20200818.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/carin-bb/fsh/ig-data/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B5D27BC-589C-564C-85F8-E54401245963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B4589A-330B-AC48-8733-A04B5FA9DC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -88,12 +88,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-added slice name</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>added slice name</t>
         </r>
       </text>
     </comment>
@@ -344,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14366" uniqueCount="1258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14372" uniqueCount="1261">
   <si>
     <t>Coverage</t>
   </si>
@@ -4308,12 +4317,21 @@
   <si>
     <t>CARIN for BB FHIR Profile</t>
   </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>drg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4523,6 +4541,19 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -7004,15 +7035,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L374" sqref="L374"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="K150" sqref="K150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7066,7 +7097,7 @@
       </c>
       <c r="L1" s="15"/>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="68">
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="68" hidden="1">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -7140,7 +7171,7 @@
         <v>Reference(Patient)</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="8" customFormat="1" ht="68">
+    <row r="4" spans="1:12" s="8" customFormat="1" ht="68" hidden="1">
       <c r="A4" s="38">
         <v>1</v>
       </c>
@@ -7177,7 +7208,7 @@
         <v>Reference(Patient)</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" ht="68">
+    <row r="5" spans="1:12" s="8" customFormat="1" ht="68" hidden="1">
       <c r="A5" s="38">
         <v>1</v>
       </c>
@@ -7214,7 +7245,7 @@
         <v>Reference(Patient)</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="8" customFormat="1" ht="68">
+    <row r="6" spans="1:12" s="8" customFormat="1" ht="68" hidden="1">
       <c r="A6" s="38">
         <v>1</v>
       </c>
@@ -7251,7 +7282,7 @@
         <v>Reference(Patient)</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" ht="46" customHeight="1">
+    <row r="7" spans="1:12" s="8" customFormat="1" ht="46" hidden="1" customHeight="1">
       <c r="A7" s="38">
         <v>2</v>
       </c>
@@ -7356,7 +7387,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="8" customFormat="1" ht="30">
+    <row r="10" spans="1:12" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A10" s="39">
         <v>2</v>
       </c>
@@ -7391,7 +7422,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="8" customFormat="1" ht="30">
+    <row r="11" spans="1:12" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A11" s="38">
         <v>2</v>
       </c>
@@ -7426,7 +7457,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="8" customFormat="1" ht="45">
+    <row r="12" spans="1:12" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A12" s="39">
         <v>2</v>
       </c>
@@ -7461,7 +7492,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="8" customFormat="1" ht="45">
+    <row r="13" spans="1:12" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A13" s="38">
         <v>2</v>
       </c>
@@ -7496,7 +7527,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="8" customFormat="1" ht="30">
+    <row r="14" spans="1:12" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A14" s="39">
         <v>2</v>
       </c>
@@ -7531,7 +7562,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="8" customFormat="1" ht="30">
+    <row r="15" spans="1:12" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A15" s="38">
         <v>2</v>
       </c>
@@ -7566,7 +7597,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="8" customFormat="1" ht="30">
+    <row r="16" spans="1:12" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A16" s="38">
         <v>3</v>
       </c>
@@ -7598,7 +7629,7 @@
       </c>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" ht="98">
+    <row r="17" spans="1:11" s="8" customFormat="1" ht="98" hidden="1">
       <c r="A17" s="38">
         <v>6</v>
       </c>
@@ -7630,7 +7661,7 @@
       </c>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="1:11" s="8" customFormat="1" ht="78" customHeight="1">
+    <row r="18" spans="1:11" s="8" customFormat="1" ht="78" hidden="1" customHeight="1">
       <c r="A18" s="38">
         <v>6</v>
       </c>
@@ -7662,7 +7693,7 @@
       </c>
       <c r="K18" s="17"/>
     </row>
-    <row r="19" spans="1:11" s="8" customFormat="1" ht="65.25" customHeight="1">
+    <row r="19" spans="1:11" s="8" customFormat="1" ht="65.25" hidden="1" customHeight="1">
       <c r="A19" s="38">
         <v>7</v>
       </c>
@@ -7696,7 +7727,7 @@
       </c>
       <c r="K19" s="17"/>
     </row>
-    <row r="20" spans="1:11" s="8" customFormat="1" ht="56">
+    <row r="20" spans="1:11" s="8" customFormat="1" ht="56" hidden="1">
       <c r="A20" s="38">
         <v>7</v>
       </c>
@@ -7730,7 +7761,7 @@
       </c>
       <c r="K20" s="17"/>
     </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="21" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A21" s="38">
         <v>7</v>
       </c>
@@ -7764,7 +7795,7 @@
       </c>
       <c r="K21" s="17"/>
     </row>
-    <row r="22" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="22" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A22" s="39">
         <v>8</v>
       </c>
@@ -7798,7 +7829,7 @@
       </c>
       <c r="K22" s="17"/>
     </row>
-    <row r="23" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="23" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A23" s="39">
         <v>8</v>
       </c>
@@ -7832,7 +7863,7 @@
       </c>
       <c r="K23" s="17"/>
     </row>
-    <row r="24" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="24" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A24" s="39">
         <v>8</v>
       </c>
@@ -7866,7 +7897,7 @@
       </c>
       <c r="K24" s="17"/>
     </row>
-    <row r="25" spans="1:11" s="8" customFormat="1" ht="84">
+    <row r="25" spans="1:11" s="8" customFormat="1" ht="84" hidden="1">
       <c r="A25" s="38">
         <v>9</v>
       </c>
@@ -7897,7 +7928,7 @@
       </c>
       <c r="K25" s="17"/>
     </row>
-    <row r="26" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="26" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A26" s="38">
         <v>10</v>
       </c>
@@ -7929,7 +7960,7 @@
       </c>
       <c r="K26" s="17"/>
     </row>
-    <row r="27" spans="1:11" s="8" customFormat="1" ht="42">
+    <row r="27" spans="1:11" s="8" customFormat="1" ht="42" hidden="1">
       <c r="A27" s="38">
         <v>11</v>
       </c>
@@ -7961,7 +7992,7 @@
       </c>
       <c r="K27" s="17"/>
     </row>
-    <row r="28" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="28" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A28" s="38">
         <v>12</v>
       </c>
@@ -8030,7 +8061,7 @@
         <v>pointoforigin</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="8" customFormat="1" ht="70">
+    <row r="30" spans="1:11" s="8" customFormat="1" ht="70" hidden="1">
       <c r="A30" s="38">
         <v>13</v>
       </c>
@@ -8110,7 +8141,7 @@
         <v>admtype</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="8" customFormat="1" ht="86.25" customHeight="1">
+    <row r="32" spans="1:11" s="8" customFormat="1" ht="86.25" hidden="1" customHeight="1">
       <c r="A32" s="38">
         <v>14</v>
       </c>
@@ -8150,7 +8181,7 @@
         <v>admtype</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="33" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A33" s="38">
         <v>15</v>
       </c>
@@ -8184,7 +8215,7 @@
       </c>
       <c r="K33" s="17"/>
     </row>
-    <row r="34" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="34" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A34" s="38">
         <v>15</v>
       </c>
@@ -8218,7 +8249,7 @@
       </c>
       <c r="K34" s="17"/>
     </row>
-    <row r="35" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="35" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A35" s="38">
         <v>15</v>
       </c>
@@ -8252,7 +8283,7 @@
       </c>
       <c r="K35" s="17"/>
     </row>
-    <row r="36" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="36" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A36" s="38">
         <v>15</v>
       </c>
@@ -8320,7 +8351,7 @@
       </c>
       <c r="K37" s="17"/>
     </row>
-    <row r="38" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="38" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A38" s="40">
         <v>16</v>
       </c>
@@ -8354,7 +8385,7 @@
       </c>
       <c r="K38" s="17"/>
     </row>
-    <row r="39" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="39" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A39" s="40">
         <v>16</v>
       </c>
@@ -8388,7 +8419,7 @@
       </c>
       <c r="K39" s="17"/>
     </row>
-    <row r="40" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="40" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A40" s="40">
         <v>16</v>
       </c>
@@ -8462,7 +8493,7 @@
         <v>typeofbill</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="8" customFormat="1" ht="98">
+    <row r="42" spans="1:11" s="8" customFormat="1" ht="98" hidden="1">
       <c r="A42" s="40">
         <v>17</v>
       </c>
@@ -8529,11 +8560,12 @@
         <f>'EOB Inpatient Institutional'!$C$100</f>
         <v>supportingInfo</v>
       </c>
-      <c r="I43" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$N$100</f>
-        <v xml:space="preserve">  </v>
-      </c>
-      <c r="J43" s="17"/>
+      <c r="I43" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="J43" s="17" t="s">
+        <v>1258</v>
+      </c>
       <c r="K43" s="17" t="str">
         <f>'EOB Inpatient Institutional'!$A$100</f>
         <v>admissionperiod</v>
@@ -8566,11 +8598,12 @@
         <f>'EOB Inpatient Institutional'!$C$100</f>
         <v>supportingInfo</v>
       </c>
-      <c r="I44" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$N$100</f>
-        <v xml:space="preserve">  </v>
-      </c>
-      <c r="J44" s="17"/>
+      <c r="I44" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>1259</v>
+      </c>
       <c r="K44" s="17" t="str">
         <f>'EOB Inpatient Institutional'!$A$100</f>
         <v>admissionperiod</v>
@@ -8656,7 +8689,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="8" customFormat="1" ht="42">
+    <row r="47" spans="1:11" s="8" customFormat="1" ht="42" hidden="1">
       <c r="A47" s="38">
         <v>20</v>
       </c>
@@ -8696,7 +8729,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="8" customFormat="1" ht="43.5" customHeight="1">
+    <row r="48" spans="1:11" s="8" customFormat="1" ht="43.5" hidden="1" customHeight="1">
       <c r="A48" s="38">
         <v>20</v>
       </c>
@@ -8736,7 +8769,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="8" customFormat="1" ht="57" customHeight="1">
+    <row r="49" spans="1:11" s="8" customFormat="1" ht="57" hidden="1" customHeight="1">
       <c r="A49" s="38">
         <v>20</v>
       </c>
@@ -8776,7 +8809,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="8" customFormat="1" ht="50.25" customHeight="1">
+    <row r="50" spans="1:11" s="8" customFormat="1" ht="50.25" hidden="1" customHeight="1">
       <c r="A50" s="38">
         <v>20</v>
       </c>
@@ -8896,7 +8929,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" ht="91" customHeight="1">
+    <row r="53" spans="1:11" s="1" customFormat="1" ht="91" hidden="1" customHeight="1">
       <c r="A53" s="38">
         <v>20</v>
       </c>
@@ -8936,7 +8969,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="100.5" customHeight="1">
+    <row r="54" spans="1:11" ht="100.5" hidden="1" customHeight="1">
       <c r="A54" s="38">
         <v>20</v>
       </c>
@@ -8976,7 +9009,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="99">
+    <row r="55" spans="1:11" ht="99" hidden="1">
       <c r="A55" s="38">
         <v>20</v>
       </c>
@@ -9016,7 +9049,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="99">
+    <row r="56" spans="1:11" ht="99" hidden="1">
       <c r="A56" s="38">
         <v>20</v>
       </c>
@@ -9134,7 +9167,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="70">
+    <row r="59" spans="1:11" ht="70" hidden="1">
       <c r="A59" s="38">
         <v>20</v>
       </c>
@@ -9172,7 +9205,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="70">
+    <row r="60" spans="1:11" ht="70" hidden="1">
       <c r="A60" s="38">
         <v>20</v>
       </c>
@@ -9212,7 +9245,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="70">
+    <row r="61" spans="1:11" ht="70" hidden="1">
       <c r="A61" s="38">
         <v>20</v>
       </c>
@@ -9252,7 +9285,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="70">
+    <row r="62" spans="1:11" ht="70" hidden="1">
       <c r="A62" s="38">
         <v>20</v>
       </c>
@@ -9372,7 +9405,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="70">
+    <row r="65" spans="1:11" ht="70" hidden="1">
       <c r="A65" s="38">
         <v>20</v>
       </c>
@@ -9412,7 +9445,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="70">
+    <row r="66" spans="1:11" ht="70" hidden="1">
       <c r="A66" s="38">
         <v>20</v>
       </c>
@@ -9452,7 +9485,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="70">
+    <row r="67" spans="1:11" ht="70" hidden="1">
       <c r="A67" s="38">
         <v>20</v>
       </c>
@@ -9492,7 +9525,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="51">
+    <row r="68" spans="1:11" ht="51" hidden="1">
       <c r="A68" s="38">
         <v>20</v>
       </c>
@@ -9608,7 +9641,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="85">
+    <row r="71" spans="1:11" ht="85" hidden="1">
       <c r="A71" s="38">
         <v>20</v>
       </c>
@@ -9646,7 +9679,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="70">
+    <row r="72" spans="1:11" ht="70" hidden="1">
       <c r="A72" s="38">
         <v>20</v>
       </c>
@@ -9684,7 +9717,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="70">
+    <row r="73" spans="1:11" ht="70" hidden="1">
       <c r="A73" s="38">
         <v>20</v>
       </c>
@@ -9722,7 +9755,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="68">
+    <row r="74" spans="1:11" ht="68" hidden="1">
       <c r="A74" s="38">
         <v>20</v>
       </c>
@@ -9840,7 +9873,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="58" customHeight="1">
+    <row r="77" spans="1:11" ht="58" hidden="1" customHeight="1">
       <c r="A77" s="38">
         <v>20</v>
       </c>
@@ -9880,7 +9913,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="102">
+    <row r="78" spans="1:11" ht="102" hidden="1">
       <c r="A78" s="38">
         <v>20</v>
       </c>
@@ -9920,7 +9953,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="102">
+    <row r="79" spans="1:11" ht="102" hidden="1">
       <c r="A79" s="38">
         <v>20</v>
       </c>
@@ -9960,7 +9993,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="102">
+    <row r="80" spans="1:11" ht="102" hidden="1">
       <c r="A80" s="38">
         <v>20</v>
       </c>
@@ -10080,7 +10113,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="34">
+    <row r="83" spans="1:11" ht="34" hidden="1">
       <c r="A83" s="38">
         <v>20</v>
       </c>
@@ -10120,7 +10153,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="45">
+    <row r="84" spans="1:11" ht="45" hidden="1">
       <c r="A84" s="38">
         <v>20</v>
       </c>
@@ -10160,7 +10193,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="45">
+    <row r="85" spans="1:11" ht="45" hidden="1">
       <c r="A85" s="38">
         <v>20</v>
       </c>
@@ -10200,7 +10233,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="45">
+    <row r="86" spans="1:11" ht="45" hidden="1">
       <c r="A86" s="38">
         <v>20</v>
       </c>
@@ -10320,7 +10353,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="98">
+    <row r="89" spans="1:11" ht="98" hidden="1">
       <c r="A89" s="38">
         <v>20</v>
       </c>
@@ -10360,7 +10393,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="98">
+    <row r="90" spans="1:11" ht="98" hidden="1">
       <c r="A90" s="38">
         <v>20</v>
       </c>
@@ -10400,7 +10433,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="98">
+    <row r="91" spans="1:11" ht="98" hidden="1">
       <c r="A91" s="38">
         <v>20</v>
       </c>
@@ -10440,7 +10473,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="98">
+    <row r="92" spans="1:11" ht="98" hidden="1">
       <c r="A92" s="38">
         <v>20</v>
       </c>
@@ -10560,7 +10593,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="30">
+    <row r="95" spans="1:11" ht="30" hidden="1">
       <c r="A95" s="38">
         <v>20</v>
       </c>
@@ -10600,7 +10633,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="45">
+    <row r="96" spans="1:11" ht="45" hidden="1">
       <c r="A96" s="38">
         <v>20</v>
       </c>
@@ -10640,7 +10673,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="45">
+    <row r="97" spans="1:11" ht="45" hidden="1">
       <c r="A97" s="38">
         <v>20</v>
       </c>
@@ -10680,7 +10713,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="107" customHeight="1">
+    <row r="98" spans="1:11" ht="107" hidden="1" customHeight="1">
       <c r="A98" s="38">
         <v>20</v>
       </c>
@@ -10796,7 +10829,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="1" customFormat="1" ht="91" customHeight="1">
+    <row r="101" spans="1:11" s="1" customFormat="1" ht="91" hidden="1" customHeight="1">
       <c r="A101" s="38">
         <v>20</v>
       </c>
@@ -10834,7 +10867,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="100.5" customHeight="1">
+    <row r="102" spans="1:11" ht="100.5" hidden="1" customHeight="1">
       <c r="A102" s="38">
         <v>20</v>
       </c>
@@ -10872,7 +10905,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="45">
+    <row r="103" spans="1:11" ht="45" hidden="1">
       <c r="A103" s="38">
         <v>20</v>
       </c>
@@ -10910,7 +10943,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="30">
+    <row r="104" spans="1:11" ht="30" hidden="1">
       <c r="A104" s="38">
         <v>20</v>
       </c>
@@ -10948,7 +10981,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="56">
+    <row r="105" spans="1:11" ht="56" hidden="1">
       <c r="A105" s="38">
         <v>20</v>
       </c>
@@ -11068,7 +11101,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="34">
+    <row r="108" spans="1:11" ht="34" hidden="1">
       <c r="A108" s="38">
         <v>20</v>
       </c>
@@ -11108,7 +11141,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="34">
+    <row r="109" spans="1:11" ht="34" hidden="1">
       <c r="A109" s="38">
         <v>20</v>
       </c>
@@ -11148,7 +11181,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="45">
+    <row r="110" spans="1:11" ht="45" hidden="1">
       <c r="A110" s="38">
         <v>20</v>
       </c>
@@ -11188,7 +11221,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="34">
+    <row r="111" spans="1:11" ht="34" hidden="1">
       <c r="A111" s="38">
         <v>20</v>
       </c>
@@ -11304,7 +11337,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="30">
+    <row r="114" spans="1:11" ht="30" hidden="1">
       <c r="A114" s="38">
         <v>20</v>
       </c>
@@ -11342,7 +11375,7 @@
         <v>Monetary amount</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="30">
+    <row r="115" spans="1:11" ht="30" hidden="1">
       <c r="A115" s="38">
         <v>20</v>
       </c>
@@ -11380,7 +11413,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="45">
+    <row r="116" spans="1:11" ht="45" hidden="1">
       <c r="A116" s="38">
         <v>20</v>
       </c>
@@ -11418,7 +11451,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="30">
+    <row r="117" spans="1:11" ht="30" hidden="1">
       <c r="A117" s="38">
         <v>20</v>
       </c>
@@ -11532,7 +11565,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="30">
+    <row r="120" spans="1:11" ht="30" hidden="1">
       <c r="A120" s="38">
         <v>20</v>
       </c>
@@ -11570,7 +11603,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="30">
+    <row r="121" spans="1:11" ht="30" hidden="1">
       <c r="A121" s="38">
         <v>20</v>
       </c>
@@ -11608,7 +11641,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="45">
+    <row r="122" spans="1:11" ht="45" hidden="1">
       <c r="A122" s="38">
         <v>20</v>
       </c>
@@ -11646,7 +11679,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30">
+    <row r="123" spans="1:11" ht="30" hidden="1">
       <c r="A123" s="38">
         <v>20</v>
       </c>
@@ -11716,7 +11749,7 @@
       </c>
       <c r="K124" s="17"/>
     </row>
-    <row r="125" spans="1:11" s="8" customFormat="1" ht="65.25" customHeight="1">
+    <row r="125" spans="1:11" s="8" customFormat="1" ht="65.25" hidden="1" customHeight="1">
       <c r="A125" s="38">
         <v>21</v>
       </c>
@@ -11782,7 +11815,7 @@
       </c>
       <c r="K126" s="17"/>
     </row>
-    <row r="127" spans="1:11" s="8" customFormat="1" ht="56">
+    <row r="127" spans="1:11" s="8" customFormat="1" ht="56" hidden="1">
       <c r="A127" s="38">
         <v>22</v>
       </c>
@@ -11816,7 +11849,7 @@
       </c>
       <c r="K127" s="17"/>
     </row>
-    <row r="128" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="128" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A128" s="38">
         <v>22</v>
       </c>
@@ -11850,7 +11883,7 @@
       </c>
       <c r="K128" s="17"/>
     </row>
-    <row r="129" spans="1:11" s="8" customFormat="1" ht="52" customHeight="1">
+    <row r="129" spans="1:11" s="8" customFormat="1" ht="52" hidden="1" customHeight="1">
       <c r="A129" s="38">
         <v>22</v>
       </c>
@@ -11918,7 +11951,7 @@
       </c>
       <c r="K130" s="17"/>
     </row>
-    <row r="131" spans="1:11" s="8" customFormat="1" ht="39" customHeight="1">
+    <row r="131" spans="1:11" s="8" customFormat="1" ht="39" hidden="1" customHeight="1">
       <c r="A131" s="38">
         <v>23</v>
       </c>
@@ -11952,7 +11985,7 @@
       </c>
       <c r="K131" s="17"/>
     </row>
-    <row r="132" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="132" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A132" s="38">
         <v>23</v>
       </c>
@@ -11986,7 +12019,7 @@
       </c>
       <c r="K132" s="17"/>
     </row>
-    <row r="133" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="133" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A133" s="38">
         <v>23</v>
       </c>
@@ -12022,247 +12055,247 @@
     </row>
     <row r="134" spans="1:11" s="8" customFormat="1" ht="70">
       <c r="A134" s="38">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B134" s="17" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>661</v>
+        <v>331</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="E134" s="17" t="s">
         <v>1223</v>
       </c>
-      <c r="F134" s="50">
+      <c r="F134" s="60">
         <v>43665</v>
       </c>
       <c r="G134" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$B$235</f>
+        <v>ExplanationOfBenefit</v>
+      </c>
+      <c r="H134" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$C$235</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="I134" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$D$235</f>
+        <v>onAdmission</v>
+      </c>
+      <c r="J134" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$J$235</f>
+        <v>Present on admission</v>
+      </c>
+      <c r="K134" s="17"/>
+    </row>
+    <row r="135" spans="1:11" s="8" customFormat="1" ht="30">
+      <c r="A135" s="38">
+        <v>29</v>
+      </c>
+      <c r="B135" s="17" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C135" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D135" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="E135" s="17" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F135" s="60">
+        <v>43665</v>
+      </c>
+      <c r="G135" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$B$235</f>
+        <v>ExplanationOfBenefit</v>
+      </c>
+      <c r="H135" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$C$235</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="I135" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$D$235</f>
+        <v>onAdmission</v>
+      </c>
+      <c r="J135" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$J$235</f>
+        <v>Present on admission</v>
+      </c>
+      <c r="K135" s="17"/>
+    </row>
+    <row r="136" spans="1:11" s="8" customFormat="1" ht="70">
+      <c r="A136" s="38">
+        <v>30</v>
+      </c>
+      <c r="B136" s="17"/>
+      <c r="C136" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="E136" s="17" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F136" s="50">
+        <v>43670</v>
+      </c>
+      <c r="G136" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$B$231</f>
+        <v>ExplanationOfBenefit</v>
+      </c>
+      <c r="H136" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$C$231</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="I136" s="17"/>
+      <c r="J136" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$J$231</f>
+        <v>ICD-10 Codes (Example)</v>
+      </c>
+      <c r="K136" s="17"/>
+    </row>
+    <row r="137" spans="1:11" s="8" customFormat="1" ht="30">
+      <c r="A137" s="38">
+        <v>31</v>
+      </c>
+      <c r="B137" s="17"/>
+      <c r="C137" s="9" t="s">
+        <v>874</v>
+      </c>
+      <c r="D137" s="18" t="s">
+        <v>544</v>
+      </c>
+      <c r="E137" s="17" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F137" s="50">
+        <v>43670</v>
+      </c>
+      <c r="G137" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$B$231</f>
+        <v>ExplanationOfBenefit</v>
+      </c>
+      <c r="H137" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$C$231</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="I137" s="17"/>
+      <c r="J137" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$J$231</f>
+        <v>ICD-10 Codes (Example)</v>
+      </c>
+      <c r="K137" s="17"/>
+    </row>
+    <row r="138" spans="1:11" s="8" customFormat="1" ht="84">
+      <c r="A138" s="38">
+        <v>145</v>
+      </c>
+      <c r="B138" s="17"/>
+      <c r="C138" s="9" t="s">
+        <v>850</v>
+      </c>
+      <c r="D138" s="61" t="s">
+        <v>851</v>
+      </c>
+      <c r="E138" s="17" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F138" s="60">
+        <v>43665</v>
+      </c>
+      <c r="G138" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$B$230</f>
+        <v>ExplanationOfBenefit</v>
+      </c>
+      <c r="H138" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$C$230</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="I138" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$D$230</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="J138" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$I$230</f>
+        <v>CodeableConcept</v>
+      </c>
+      <c r="K138" s="17"/>
+    </row>
+    <row r="139" spans="1:11" s="8" customFormat="1" ht="84">
+      <c r="A139" s="38">
+        <v>146</v>
+      </c>
+      <c r="B139" s="17"/>
+      <c r="C139" s="9" t="s">
+        <v>855</v>
+      </c>
+      <c r="D139" s="61" t="s">
+        <v>856</v>
+      </c>
+      <c r="E139" s="17" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F139" s="54">
+        <v>43665</v>
+      </c>
+      <c r="G139" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$B$230</f>
+        <v>ExplanationOfBenefit</v>
+      </c>
+      <c r="H139" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$C$230</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="I139" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$D$230</f>
+        <v>diagnosis</v>
+      </c>
+      <c r="J139" s="17" t="str">
+        <f>'EOB Inpatient Institutional'!$I$230</f>
+        <v>CodeableConcept</v>
+      </c>
+      <c r="K139" s="17"/>
+    </row>
+    <row r="140" spans="1:11" s="8" customFormat="1" ht="66" customHeight="1">
+      <c r="A140" s="38">
+        <v>24</v>
+      </c>
+      <c r="B140" s="17" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="E140" s="17" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F140" s="50">
+        <v>43665</v>
+      </c>
+      <c r="G140" s="17" t="str">
         <f>'EOB Inpatient Institutional'!$B$244</f>
         <v>ExplanationOfBenefit</v>
       </c>
-      <c r="H134" s="17" t="str">
+      <c r="H140" s="17" t="str">
         <f>'EOB Inpatient Institutional'!$C$244</f>
         <v>procedure</v>
       </c>
-      <c r="I134" s="17"/>
-      <c r="J134" s="17" t="str">
+      <c r="I140" s="17"/>
+      <c r="J140" s="17" t="str">
         <f>'EOB Inpatient Institutional'!$J$244</f>
         <v>Specific clinical procedure</v>
       </c>
-      <c r="K134" s="17"/>
-    </row>
-    <row r="135" spans="1:11" s="8" customFormat="1" ht="30">
-      <c r="A135" s="38">
-        <v>25</v>
-      </c>
-      <c r="B135" s="17" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C135" s="9" t="s">
-        <v>657</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="E135" s="17" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F135" s="50">
-        <v>43665</v>
-      </c>
-      <c r="G135" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$243</f>
-        <v>ExplanationOfBenefit</v>
-      </c>
-      <c r="H135" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$243</f>
-        <v>procedure</v>
-      </c>
-      <c r="I135" s="17"/>
-      <c r="J135" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$J$243</f>
-        <v>When the procedure was performed</v>
-      </c>
-      <c r="K135" s="17"/>
-    </row>
-    <row r="136" spans="1:11" s="8" customFormat="1" ht="70">
-      <c r="A136" s="38">
-        <v>26</v>
-      </c>
-      <c r="B136" s="17" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C136" s="9" t="s">
-        <v>662</v>
-      </c>
-      <c r="D136" s="9" t="s">
-        <v>540</v>
-      </c>
-      <c r="E136" s="17" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F136" s="50">
-        <v>43665</v>
-      </c>
-      <c r="G136" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$244</f>
-        <v>ExplanationOfBenefit</v>
-      </c>
-      <c r="H136" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$244</f>
-        <v>procedure</v>
-      </c>
-      <c r="I136" s="17"/>
-      <c r="J136" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$J$244</f>
-        <v>Specific clinical procedure</v>
-      </c>
-      <c r="K136" s="17"/>
-    </row>
-    <row r="137" spans="1:11" s="8" customFormat="1" ht="30">
-      <c r="A137" s="38">
-        <v>27</v>
-      </c>
-      <c r="B137" s="17" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>658</v>
-      </c>
-      <c r="D137" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="E137" s="17" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F137" s="50">
-        <v>43665</v>
-      </c>
-      <c r="G137" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$243</f>
-        <v>ExplanationOfBenefit</v>
-      </c>
-      <c r="H137" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$243</f>
-        <v>procedure</v>
-      </c>
-      <c r="I137" s="17"/>
-      <c r="J137" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$J$243</f>
-        <v>When the procedure was performed</v>
-      </c>
-      <c r="K137" s="17"/>
-    </row>
-    <row r="138" spans="1:11" s="8" customFormat="1" ht="84">
-      <c r="A138" s="38">
-        <v>28</v>
-      </c>
-      <c r="B138" s="17" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C138" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="D138" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="E138" s="17" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F138" s="60">
-        <v>43665</v>
-      </c>
-      <c r="G138" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$235</f>
-        <v>ExplanationOfBenefit</v>
-      </c>
-      <c r="H138" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$235</f>
-        <v>diagnosis</v>
-      </c>
-      <c r="I138" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$D$235</f>
-        <v>onAdmission</v>
-      </c>
-      <c r="J138" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$J$235</f>
-        <v>Present on admission</v>
-      </c>
-      <c r="K138" s="17"/>
-    </row>
-    <row r="139" spans="1:11" s="8" customFormat="1" ht="84">
-      <c r="A139" s="38">
-        <v>29</v>
-      </c>
-      <c r="B139" s="17" t="s">
-        <v>1210</v>
-      </c>
-      <c r="C139" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="D139" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="E139" s="17" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F139" s="60">
-        <v>43665</v>
-      </c>
-      <c r="G139" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$235</f>
-        <v>ExplanationOfBenefit</v>
-      </c>
-      <c r="H139" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$235</f>
-        <v>diagnosis</v>
-      </c>
-      <c r="I139" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$D$235</f>
-        <v>onAdmission</v>
-      </c>
-      <c r="J139" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$J$235</f>
-        <v>Present on admission</v>
-      </c>
-      <c r="K139" s="17"/>
-    </row>
-    <row r="140" spans="1:11" s="8" customFormat="1" ht="66" customHeight="1">
-      <c r="A140" s="38">
-        <v>30</v>
-      </c>
-      <c r="B140" s="17"/>
-      <c r="C140" s="9" t="s">
-        <v>647</v>
-      </c>
-      <c r="D140" s="9" t="s">
-        <v>543</v>
-      </c>
-      <c r="E140" s="17" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F140" s="50">
-        <v>43670</v>
-      </c>
-      <c r="G140" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$231</f>
-        <v>ExplanationOfBenefit</v>
-      </c>
-      <c r="H140" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$231</f>
-        <v>diagnosis</v>
-      </c>
-      <c r="I140" s="17"/>
-      <c r="J140" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$J$231</f>
-        <v>ICD-10 Codes (Example)</v>
-      </c>
       <c r="K140" s="17"/>
     </row>
-    <row r="141" spans="1:11" s="8" customFormat="1" ht="43.5" customHeight="1">
+    <row r="141" spans="1:11" s="8" customFormat="1" ht="43.5" hidden="1" customHeight="1">
       <c r="A141" s="38">
         <v>30</v>
       </c>
@@ -12296,37 +12329,39 @@
     </row>
     <row r="142" spans="1:11" s="8" customFormat="1" ht="97.5" customHeight="1">
       <c r="A142" s="38">
-        <v>31</v>
-      </c>
-      <c r="B142" s="17"/>
+        <v>25</v>
+      </c>
+      <c r="B142" s="17" t="s">
+        <v>1213</v>
+      </c>
       <c r="C142" s="9" t="s">
-        <v>874</v>
-      </c>
-      <c r="D142" s="18" t="s">
-        <v>544</v>
+        <v>657</v>
+      </c>
+      <c r="D142" s="9" t="s">
+        <v>539</v>
       </c>
       <c r="E142" s="17" t="s">
         <v>1223</v>
       </c>
       <c r="F142" s="50">
-        <v>43670</v>
+        <v>43665</v>
       </c>
       <c r="G142" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$231</f>
+        <f>'EOB Inpatient Institutional'!$B$243</f>
         <v>ExplanationOfBenefit</v>
       </c>
       <c r="H142" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$231</f>
-        <v>diagnosis</v>
+        <f>'EOB Inpatient Institutional'!$C$243</f>
+        <v>procedure</v>
       </c>
       <c r="I142" s="17"/>
       <c r="J142" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$J$231</f>
-        <v>ICD-10 Codes (Example)</v>
+        <f>'EOB Inpatient Institutional'!$J$243</f>
+        <v>When the procedure was performed</v>
       </c>
       <c r="K142" s="17"/>
     </row>
-    <row r="143" spans="1:11" s="8" customFormat="1" ht="84">
+    <row r="143" spans="1:11" s="8" customFormat="1" ht="84" hidden="1">
       <c r="A143" s="38">
         <v>31</v>
       </c>
@@ -12393,9 +12428,8 @@
         <f>'EOB Inpatient Institutional'!$J$198</f>
         <v>Classification of the supplied information</v>
       </c>
-      <c r="K144" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$A$198</f>
-        <v>DRG</v>
+      <c r="K144" s="17" t="s">
+        <v>1260</v>
       </c>
     </row>
     <row r="145" spans="1:11" s="8" customFormat="1" ht="30">
@@ -12433,12 +12467,11 @@
         <f>'EOB Inpatient Institutional'!$J$198</f>
         <v>Classification of the supplied information</v>
       </c>
-      <c r="K145" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$A$198</f>
-        <v>DRG</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" s="8" customFormat="1" ht="30">
+      <c r="K145" s="17" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A146" s="38">
         <v>34</v>
       </c>
@@ -12475,7 +12508,7 @@
       </c>
       <c r="K146" s="17"/>
     </row>
-    <row r="147" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="147" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A147" s="38">
         <v>34</v>
       </c>
@@ -12512,7 +12545,7 @@
       </c>
       <c r="K147" s="17"/>
     </row>
-    <row r="148" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="148" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A148" s="38">
         <v>34</v>
       </c>
@@ -12549,7 +12582,7 @@
       </c>
       <c r="K148" s="17"/>
     </row>
-    <row r="149" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="149" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A149" s="38">
         <v>34</v>
       </c>
@@ -12620,7 +12653,7 @@
       </c>
       <c r="K150" s="17"/>
     </row>
-    <row r="151" spans="1:11" s="8" customFormat="1" ht="84">
+    <row r="151" spans="1:11" s="8" customFormat="1" ht="84" hidden="1">
       <c r="A151" s="38">
         <v>35</v>
       </c>
@@ -12654,7 +12687,7 @@
       </c>
       <c r="K151" s="17"/>
     </row>
-    <row r="152" spans="1:11" s="8" customFormat="1" ht="92.5" customHeight="1">
+    <row r="152" spans="1:11" s="8" customFormat="1" ht="92.5" hidden="1" customHeight="1">
       <c r="A152" s="38">
         <v>35</v>
       </c>
@@ -12688,7 +12721,7 @@
       </c>
       <c r="K152" s="17"/>
     </row>
-    <row r="153" spans="1:11" s="8" customFormat="1" ht="42">
+    <row r="153" spans="1:11" s="8" customFormat="1" ht="42" hidden="1">
       <c r="A153" s="38">
         <v>35</v>
       </c>
@@ -12759,7 +12792,7 @@
       </c>
       <c r="K154" s="17"/>
     </row>
-    <row r="155" spans="1:11" s="8" customFormat="1" ht="42">
+    <row r="155" spans="1:11" s="8" customFormat="1" ht="42" hidden="1">
       <c r="A155" s="38">
         <v>36</v>
       </c>
@@ -12796,7 +12829,7 @@
       </c>
       <c r="K155" s="17"/>
     </row>
-    <row r="156" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="156" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A156" s="38">
         <v>36</v>
       </c>
@@ -12833,7 +12866,7 @@
       </c>
       <c r="K156" s="17"/>
     </row>
-    <row r="157" spans="1:11" s="8" customFormat="1" ht="42">
+    <row r="157" spans="1:11" s="8" customFormat="1" ht="42" hidden="1">
       <c r="A157" s="38">
         <v>36</v>
       </c>
@@ -12870,7 +12903,7 @@
       </c>
       <c r="K157" s="17"/>
     </row>
-    <row r="158" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="158" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A158" s="38">
         <v>38</v>
       </c>
@@ -12907,7 +12940,7 @@
       </c>
       <c r="K158" s="17"/>
     </row>
-    <row r="159" spans="1:11" s="8" customFormat="1" ht="60">
+    <row r="159" spans="1:11" s="8" customFormat="1" ht="60" hidden="1">
       <c r="A159" s="38">
         <v>39</v>
       </c>
@@ -12979,7 +13012,7 @@
       </c>
       <c r="K160" s="17"/>
     </row>
-    <row r="161" spans="1:11" s="8" customFormat="1" ht="56">
+    <row r="161" spans="1:11" s="8" customFormat="1" ht="56" hidden="1">
       <c r="A161" s="38">
         <v>40</v>
       </c>
@@ -13014,7 +13047,7 @@
       </c>
       <c r="K161" s="17"/>
     </row>
-    <row r="162" spans="1:11" s="8" customFormat="1" ht="56">
+    <row r="162" spans="1:11" s="8" customFormat="1" ht="56" hidden="1">
       <c r="A162" s="41">
         <v>40</v>
       </c>
@@ -13086,7 +13119,7 @@
       </c>
       <c r="K163" s="17"/>
     </row>
-    <row r="164" spans="1:11" s="8" customFormat="1" ht="42">
+    <row r="164" spans="1:11" s="8" customFormat="1" ht="42" hidden="1">
       <c r="A164" s="38">
         <v>41</v>
       </c>
@@ -13123,7 +13156,7 @@
       </c>
       <c r="K164" s="17"/>
     </row>
-    <row r="165" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="165" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A165" s="38">
         <v>41</v>
       </c>
@@ -13197,7 +13230,7 @@
       </c>
       <c r="K166" s="17"/>
     </row>
-    <row r="167" spans="1:11" s="8" customFormat="1" ht="52" customHeight="1">
+    <row r="167" spans="1:11" s="8" customFormat="1" ht="52" hidden="1" customHeight="1">
       <c r="A167" s="38">
         <v>42</v>
       </c>
@@ -13234,7 +13267,7 @@
       </c>
       <c r="K167" s="17"/>
     </row>
-    <row r="168" spans="1:11" s="8" customFormat="1" ht="56">
+    <row r="168" spans="1:11" s="8" customFormat="1" ht="56" hidden="1">
       <c r="A168" s="38">
         <v>42</v>
       </c>
@@ -13271,7 +13304,7 @@
       </c>
       <c r="K168" s="17"/>
     </row>
-    <row r="169" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="169" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A169" s="38">
         <v>46</v>
       </c>
@@ -13308,7 +13341,7 @@
       </c>
       <c r="K169" s="17"/>
     </row>
-    <row r="170" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="170" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A170" s="38">
         <v>46</v>
       </c>
@@ -13345,7 +13378,7 @@
       </c>
       <c r="K170" s="17"/>
     </row>
-    <row r="171" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="171" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A171" s="38">
         <v>46</v>
       </c>
@@ -13382,7 +13415,7 @@
       </c>
       <c r="K171" s="17"/>
     </row>
-    <row r="172" spans="1:11" s="8" customFormat="1" ht="56">
+    <row r="172" spans="1:11" s="8" customFormat="1" ht="56" hidden="1">
       <c r="A172" s="38">
         <v>47</v>
       </c>
@@ -13420,7 +13453,7 @@
         <v>CodeableConcept</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="30">
+    <row r="173" spans="1:11" ht="30" hidden="1">
       <c r="A173" s="38">
         <v>70</v>
       </c>
@@ -13454,7 +13487,7 @@
       </c>
       <c r="K173" s="22"/>
     </row>
-    <row r="174" spans="1:11" ht="30">
+    <row r="174" spans="1:11" ht="30" hidden="1">
       <c r="A174" s="38">
         <v>71</v>
       </c>
@@ -13488,7 +13521,7 @@
       </c>
       <c r="K174" s="22"/>
     </row>
-    <row r="175" spans="1:11" ht="30">
+    <row r="175" spans="1:11" ht="30" hidden="1">
       <c r="A175" s="38">
         <v>72</v>
       </c>
@@ -13520,7 +13553,7 @@
       </c>
       <c r="K175" s="17"/>
     </row>
-    <row r="176" spans="1:11" ht="30">
+    <row r="176" spans="1:11" ht="30" hidden="1">
       <c r="A176" s="38">
         <v>74</v>
       </c>
@@ -13552,7 +13585,7 @@
       </c>
       <c r="K176" s="17"/>
     </row>
-    <row r="177" spans="1:11" ht="30">
+    <row r="177" spans="1:11" ht="30" hidden="1">
       <c r="A177" s="39">
         <v>75</v>
       </c>
@@ -13584,7 +13617,7 @@
       </c>
       <c r="K177" s="17"/>
     </row>
-    <row r="178" spans="1:11" ht="30">
+    <row r="178" spans="1:11" ht="30" hidden="1">
       <c r="A178" s="38">
         <v>77</v>
       </c>
@@ -13624,7 +13657,7 @@
         <v>dayssupply</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="30">
+    <row r="179" spans="1:11" ht="30" hidden="1">
       <c r="A179" s="38">
         <v>78</v>
       </c>
@@ -13661,7 +13694,7 @@
       </c>
       <c r="K179" s="17"/>
     </row>
-    <row r="180" spans="1:11" ht="60">
+    <row r="180" spans="1:11" ht="60" hidden="1">
       <c r="A180" s="38">
         <v>79</v>
       </c>
@@ -13701,7 +13734,7 @@
         <v>dawcode</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="56">
+    <row r="181" spans="1:11" ht="56" hidden="1">
       <c r="A181" s="38">
         <v>80</v>
       </c>
@@ -13739,7 +13772,7 @@
         <v>dispensingstatus</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="30">
+    <row r="182" spans="1:11" ht="30" hidden="1">
       <c r="A182" s="38">
         <v>85</v>
       </c>
@@ -13799,7 +13832,7 @@
       </c>
       <c r="K183" s="17"/>
     </row>
-    <row r="184" spans="1:11" ht="70">
+    <row r="184" spans="1:11" ht="70" hidden="1">
       <c r="A184" s="38">
         <v>86</v>
       </c>
@@ -13876,7 +13909,7 @@
         <v>claimrecvddate</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="30">
+    <row r="186" spans="1:11" ht="30" hidden="1">
       <c r="A186" s="38">
         <v>88</v>
       </c>
@@ -13916,7 +13949,7 @@
         <v>claimrecvddate</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="45">
+    <row r="187" spans="1:11" ht="45" hidden="1">
       <c r="A187" s="38">
         <v>88</v>
       </c>
@@ -13956,7 +13989,7 @@
         <v>claimrecvddate</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="16">
+    <row r="188" spans="1:11" ht="16" hidden="1">
       <c r="A188" s="38">
         <v>88</v>
       </c>
@@ -13996,7 +14029,7 @@
         <v>claimrecvddate</v>
       </c>
     </row>
-    <row r="189" spans="1:11" s="8" customFormat="1" ht="41.5" customHeight="1">
+    <row r="189" spans="1:11" s="8" customFormat="1" ht="41.5" hidden="1" customHeight="1">
       <c r="A189" s="38">
         <v>90</v>
       </c>
@@ -14033,7 +14066,7 @@
       </c>
       <c r="K189" s="17"/>
     </row>
-    <row r="190" spans="1:11" s="8" customFormat="1" ht="39" customHeight="1">
+    <row r="190" spans="1:11" s="8" customFormat="1" ht="39" hidden="1" customHeight="1">
       <c r="A190" s="38">
         <v>90</v>
       </c>
@@ -14105,7 +14138,7 @@
       </c>
       <c r="K191" s="17"/>
     </row>
-    <row r="192" spans="1:11" ht="30">
+    <row r="192" spans="1:11" ht="30" hidden="1">
       <c r="A192" s="38">
         <v>91</v>
       </c>
@@ -14140,7 +14173,7 @@
       </c>
       <c r="K192" s="17"/>
     </row>
-    <row r="193" spans="1:11" ht="45">
+    <row r="193" spans="1:11" ht="45" hidden="1">
       <c r="A193" s="38">
         <v>91</v>
       </c>
@@ -14175,7 +14208,7 @@
       </c>
       <c r="K193" s="17"/>
     </row>
-    <row r="194" spans="1:11" ht="30">
+    <row r="194" spans="1:11" ht="30" hidden="1">
       <c r="A194" s="38">
         <v>91</v>
       </c>
@@ -14285,7 +14318,7 @@
         <v>denialreason</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="45">
+    <row r="197" spans="1:11" ht="45" hidden="1">
       <c r="A197" s="38">
         <v>92</v>
       </c>
@@ -14323,7 +14356,7 @@
         <v>denialreason</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="45">
+    <row r="198" spans="1:11" ht="45" hidden="1">
       <c r="A198" s="38">
         <v>92</v>
       </c>
@@ -14360,7 +14393,7 @@
         <v>denialreason</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="45">
+    <row r="199" spans="1:11" ht="45" hidden="1">
       <c r="A199" s="38">
         <v>92</v>
       </c>
@@ -14397,7 +14430,7 @@
         <v>denialreason</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="45">
+    <row r="200" spans="1:11" ht="45" hidden="1">
       <c r="A200" s="38">
         <v>92</v>
       </c>
@@ -14474,7 +14507,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="52.5" customHeight="1">
+    <row r="202" spans="1:11" ht="52.5" hidden="1" customHeight="1">
       <c r="A202" s="38">
         <v>93</v>
       </c>
@@ -14551,7 +14584,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="30">
+    <row r="204" spans="1:11" ht="30" hidden="1">
       <c r="A204" s="38">
         <v>94</v>
       </c>
@@ -14588,7 +14621,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="45">
+    <row r="205" spans="1:11" ht="45" hidden="1">
       <c r="A205" s="38">
         <v>94</v>
       </c>
@@ -14625,7 +14658,7 @@
         <v>Reference(Practitioner | Organization)</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="67" customHeight="1">
+    <row r="206" spans="1:11" ht="67" hidden="1" customHeight="1">
       <c r="A206" s="38">
         <v>94</v>
       </c>
@@ -14662,7 +14695,7 @@
         <v>Reference(Practitioner | Organization)</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="71">
+    <row r="207" spans="1:11" ht="71" hidden="1">
       <c r="A207" s="38">
         <v>95</v>
       </c>
@@ -14740,7 +14773,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="209" spans="1:11" ht="46.5" customHeight="1">
+    <row r="209" spans="1:11" ht="46.5" hidden="1" customHeight="1">
       <c r="A209" s="38">
         <v>96</v>
       </c>
@@ -14778,7 +14811,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="210" spans="1:11" ht="45">
+    <row r="210" spans="1:11" ht="45" hidden="1">
       <c r="A210" s="38">
         <v>96</v>
       </c>
@@ -14816,7 +14849,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="211" spans="1:11" ht="30">
+    <row r="211" spans="1:11" ht="30" hidden="1">
       <c r="A211" s="38">
         <v>95</v>
       </c>
@@ -14854,7 +14887,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="212" spans="1:11" ht="85">
+    <row r="212" spans="1:11" ht="85" hidden="1">
       <c r="A212" s="38">
         <v>97</v>
       </c>
@@ -14934,7 +14967,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="214" spans="1:11" ht="55" customHeight="1">
+    <row r="214" spans="1:11" ht="55" hidden="1" customHeight="1">
       <c r="A214" s="38">
         <v>98</v>
       </c>
@@ -15014,7 +15047,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="216" spans="1:11" ht="34">
+    <row r="216" spans="1:11" ht="34" hidden="1">
       <c r="A216" s="38">
         <v>99</v>
       </c>
@@ -15054,7 +15087,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="217" spans="1:11" ht="45">
+    <row r="217" spans="1:11" ht="45" hidden="1">
       <c r="A217" s="38">
         <v>99</v>
       </c>
@@ -15132,7 +15165,7 @@
         <v>billingnetworkcontractingstatus</v>
       </c>
     </row>
-    <row r="219" spans="1:11" ht="57">
+    <row r="219" spans="1:11" ht="57" hidden="1">
       <c r="A219" s="38">
         <v>101</v>
       </c>
@@ -15170,7 +15203,7 @@
         <v>billingnetworkcontractingstatus</v>
       </c>
     </row>
-    <row r="220" spans="1:11" ht="57">
+    <row r="220" spans="1:11" ht="57" hidden="1">
       <c r="A220" s="38">
         <v>101</v>
       </c>
@@ -15208,7 +15241,7 @@
         <v>billingnetworkcontractingstatus</v>
       </c>
     </row>
-    <row r="221" spans="1:11" ht="57">
+    <row r="221" spans="1:11" ht="57" hidden="1">
       <c r="A221" s="38">
         <v>101</v>
       </c>
@@ -15246,7 +15279,7 @@
         <v>billingnetworkcontractingstatus</v>
       </c>
     </row>
-    <row r="222" spans="1:11" ht="57">
+    <row r="222" spans="1:11" ht="57" hidden="1">
       <c r="A222" s="38">
         <v>101</v>
       </c>
@@ -15321,7 +15354,7 @@
       </c>
       <c r="K223" s="17"/>
     </row>
-    <row r="224" spans="1:11" ht="30">
+    <row r="224" spans="1:11" ht="30" hidden="1">
       <c r="A224" s="38">
         <v>107</v>
       </c>
@@ -15358,7 +15391,7 @@
       </c>
       <c r="K224" s="17"/>
     </row>
-    <row r="225" spans="1:11" ht="45">
+    <row r="225" spans="1:11" ht="45" hidden="1">
       <c r="A225" s="38">
         <v>107</v>
       </c>
@@ -15395,7 +15428,7 @@
       </c>
       <c r="K225" s="17"/>
     </row>
-    <row r="226" spans="1:11" ht="30">
+    <row r="226" spans="1:11" ht="30" hidden="1">
       <c r="A226" s="38">
         <v>107</v>
       </c>
@@ -15467,7 +15500,7 @@
         <v>identifier</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="30">
+    <row r="228" spans="1:11" ht="30" hidden="1">
       <c r="A228" s="38">
         <v>109</v>
       </c>
@@ -15502,7 +15535,7 @@
         <v>identifier</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="45">
+    <row r="229" spans="1:11" ht="45" hidden="1">
       <c r="A229" s="38">
         <v>109</v>
       </c>
@@ -15572,7 +15605,7 @@
         <v>identifier</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="30">
+    <row r="231" spans="1:11" ht="30" hidden="1">
       <c r="A231" s="38">
         <v>110</v>
       </c>
@@ -15607,7 +15640,7 @@
         <v>identifier</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="45">
+    <row r="232" spans="1:11" ht="45" hidden="1">
       <c r="A232" s="38">
         <v>110</v>
       </c>
@@ -15674,7 +15707,7 @@
       </c>
       <c r="K233" s="17"/>
     </row>
-    <row r="234" spans="1:11" ht="56">
+    <row r="234" spans="1:11" ht="56" hidden="1">
       <c r="A234" s="38">
         <v>111</v>
       </c>
@@ -15706,7 +15739,7 @@
       </c>
       <c r="K234" s="17"/>
     </row>
-    <row r="235" spans="1:11" ht="56">
+    <row r="235" spans="1:11" ht="56" hidden="1">
       <c r="A235" s="38">
         <v>111</v>
       </c>
@@ -15738,7 +15771,7 @@
       </c>
       <c r="K235" s="17"/>
     </row>
-    <row r="236" spans="1:11" ht="56">
+    <row r="236" spans="1:11" ht="56" hidden="1">
       <c r="A236" s="38">
         <v>111</v>
       </c>
@@ -15802,7 +15835,7 @@
       </c>
       <c r="K237" s="17"/>
     </row>
-    <row r="238" spans="1:11" ht="42">
+    <row r="238" spans="1:11" ht="42" hidden="1">
       <c r="A238" s="38">
         <v>112</v>
       </c>
@@ -15834,7 +15867,7 @@
       </c>
       <c r="K238" s="17"/>
     </row>
-    <row r="239" spans="1:11" ht="45">
+    <row r="239" spans="1:11" ht="45" hidden="1">
       <c r="A239" s="38">
         <v>112</v>
       </c>
@@ -15866,7 +15899,7 @@
       </c>
       <c r="K239" s="17"/>
     </row>
-    <row r="240" spans="1:11" ht="42">
+    <row r="240" spans="1:11" ht="42" hidden="1">
       <c r="A240" s="38">
         <v>112</v>
       </c>
@@ -15938,7 +15971,7 @@
         <v>DRG</v>
       </c>
     </row>
-    <row r="242" spans="1:11" ht="118.5" customHeight="1">
+    <row r="242" spans="1:11" ht="118.5" hidden="1" customHeight="1">
       <c r="A242" s="38">
         <v>114</v>
       </c>
@@ -15961,7 +15994,7 @@
       <c r="J242" s="17"/>
       <c r="K242" s="17"/>
     </row>
-    <row r="243" spans="1:11" ht="75">
+    <row r="243" spans="1:11" ht="75" hidden="1">
       <c r="A243" s="38">
         <v>114</v>
       </c>
@@ -15984,7 +16017,7 @@
       <c r="J243" s="17"/>
       <c r="K243" s="17"/>
     </row>
-    <row r="244" spans="1:11" ht="75">
+    <row r="244" spans="1:11" ht="75" hidden="1">
       <c r="A244" s="38">
         <v>115</v>
       </c>
@@ -16007,7 +16040,7 @@
       <c r="J244" s="17"/>
       <c r="K244" s="17"/>
     </row>
-    <row r="245" spans="1:11" ht="75">
+    <row r="245" spans="1:11" ht="75" hidden="1">
       <c r="A245" s="38">
         <v>115</v>
       </c>
@@ -16030,7 +16063,7 @@
       <c r="J245" s="17"/>
       <c r="K245" s="17"/>
     </row>
-    <row r="246" spans="1:11" ht="75">
+    <row r="246" spans="1:11" ht="75" hidden="1">
       <c r="A246" s="38">
         <v>116</v>
       </c>
@@ -16053,7 +16086,7 @@
       <c r="J246" s="17"/>
       <c r="K246" s="17"/>
     </row>
-    <row r="247" spans="1:11" ht="75">
+    <row r="247" spans="1:11" ht="75" hidden="1">
       <c r="A247" s="38">
         <v>116</v>
       </c>
@@ -16116,7 +16149,7 @@
         <v>discharge-status</v>
       </c>
     </row>
-    <row r="249" spans="1:11" ht="42">
+    <row r="249" spans="1:11" ht="42" hidden="1">
       <c r="A249" s="38">
         <v>117</v>
       </c>
@@ -16156,7 +16189,7 @@
         <v>discharge-status</v>
       </c>
     </row>
-    <row r="250" spans="1:11" s="8" customFormat="1" ht="54" customHeight="1">
+    <row r="250" spans="1:11" s="8" customFormat="1" ht="54" hidden="1" customHeight="1">
       <c r="A250" s="38">
         <v>118</v>
       </c>
@@ -16193,7 +16226,7 @@
       </c>
       <c r="K250" s="17"/>
     </row>
-    <row r="251" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="251" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A251" s="38">
         <v>119</v>
       </c>
@@ -16265,7 +16298,7 @@
       </c>
       <c r="K252" s="17"/>
     </row>
-    <row r="253" spans="1:11" ht="60">
+    <row r="253" spans="1:11" ht="60" hidden="1">
       <c r="A253" s="38">
         <v>120</v>
       </c>
@@ -16300,7 +16333,7 @@
       </c>
       <c r="K253" s="17"/>
     </row>
-    <row r="254" spans="1:11" ht="60">
+    <row r="254" spans="1:11" ht="60" hidden="1">
       <c r="A254" s="38">
         <v>120</v>
       </c>
@@ -16335,7 +16368,7 @@
       </c>
       <c r="K254" s="17"/>
     </row>
-    <row r="255" spans="1:11" ht="60">
+    <row r="255" spans="1:11" ht="60" hidden="1">
       <c r="A255" s="38">
         <v>120</v>
       </c>
@@ -16408,7 +16441,7 @@
         <v>Reference(Organization | Practioner | Patient)</v>
       </c>
     </row>
-    <row r="257" spans="1:11" ht="45">
+    <row r="257" spans="1:11" ht="45" hidden="1">
       <c r="A257" s="38">
         <v>121</v>
       </c>
@@ -16446,7 +16479,7 @@
         <v>Reference(Organization | Practioner | Patient)</v>
       </c>
     </row>
-    <row r="258" spans="1:11" ht="45">
+    <row r="258" spans="1:11" ht="45" hidden="1">
       <c r="A258" s="38">
         <v>121</v>
       </c>
@@ -16484,7 +16517,7 @@
         <v>Reference(Organization | Practioner | Patient)</v>
       </c>
     </row>
-    <row r="259" spans="1:11" ht="45">
+    <row r="259" spans="1:11" ht="45" hidden="1">
       <c r="A259" s="38">
         <v>121</v>
       </c>
@@ -16522,7 +16555,7 @@
         <v>Reference(Organization | Practioner | Patient)</v>
       </c>
     </row>
-    <row r="260" spans="1:11" ht="70">
+    <row r="260" spans="1:11" ht="70" hidden="1">
       <c r="A260" s="38">
         <v>122</v>
       </c>
@@ -16560,7 +16593,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="261" spans="1:11" ht="30">
+    <row r="261" spans="1:11" ht="30" hidden="1">
       <c r="A261" s="38">
         <v>123</v>
       </c>
@@ -16583,7 +16616,7 @@
       <c r="J261" s="17"/>
       <c r="K261" s="17"/>
     </row>
-    <row r="262" spans="1:11" ht="30">
+    <row r="262" spans="1:11" ht="30" hidden="1">
       <c r="A262" s="38">
         <v>124</v>
       </c>
@@ -16618,7 +16651,7 @@
       </c>
       <c r="K262" s="17"/>
     </row>
-    <row r="263" spans="1:11" ht="30">
+    <row r="263" spans="1:11" ht="30" hidden="1">
       <c r="A263" s="38">
         <v>125</v>
       </c>
@@ -16652,7 +16685,7 @@
       </c>
       <c r="K263" s="22"/>
     </row>
-    <row r="264" spans="1:11" ht="30">
+    <row r="264" spans="1:11" ht="30" hidden="1">
       <c r="A264" s="38">
         <v>126</v>
       </c>
@@ -16686,7 +16719,7 @@
       </c>
       <c r="K264" s="22"/>
     </row>
-    <row r="265" spans="1:11" ht="30">
+    <row r="265" spans="1:11" ht="30" hidden="1">
       <c r="A265" s="38">
         <v>127</v>
       </c>
@@ -16718,7 +16751,7 @@
       </c>
       <c r="K265" s="22"/>
     </row>
-    <row r="266" spans="1:11" ht="30">
+    <row r="266" spans="1:11" ht="30" hidden="1">
       <c r="A266" s="38">
         <v>128</v>
       </c>
@@ -16752,7 +16785,7 @@
       </c>
       <c r="K266" s="22"/>
     </row>
-    <row r="267" spans="1:11" ht="30">
+    <row r="267" spans="1:11" ht="30" hidden="1">
       <c r="A267" s="38">
         <v>129</v>
       </c>
@@ -16784,7 +16817,7 @@
       </c>
       <c r="K267" s="22"/>
     </row>
-    <row r="268" spans="1:11" ht="30">
+    <row r="268" spans="1:11" ht="30" hidden="1">
       <c r="A268" s="38">
         <v>130</v>
       </c>
@@ -16816,7 +16849,7 @@
       </c>
       <c r="K268" s="22"/>
     </row>
-    <row r="269" spans="1:11" ht="30">
+    <row r="269" spans="1:11" ht="30" hidden="1">
       <c r="A269" s="38">
         <v>131</v>
       </c>
@@ -16850,7 +16883,7 @@
       </c>
       <c r="K269" s="22"/>
     </row>
-    <row r="270" spans="1:11" ht="30">
+    <row r="270" spans="1:11" ht="30" hidden="1">
       <c r="A270" s="38">
         <v>132</v>
       </c>
@@ -16882,7 +16915,7 @@
       </c>
       <c r="K270" s="22"/>
     </row>
-    <row r="271" spans="1:11" ht="42.75" customHeight="1">
+    <row r="271" spans="1:11" ht="42.75" hidden="1" customHeight="1">
       <c r="A271" s="38">
         <v>133</v>
       </c>
@@ -16914,7 +16947,7 @@
       </c>
       <c r="K271" s="22"/>
     </row>
-    <row r="272" spans="1:11" ht="30">
+    <row r="272" spans="1:11" ht="30" hidden="1">
       <c r="A272" s="38">
         <v>134</v>
       </c>
@@ -16949,7 +16982,7 @@
       </c>
       <c r="K272" s="22"/>
     </row>
-    <row r="273" spans="1:11" ht="45">
+    <row r="273" spans="1:11" ht="45" hidden="1">
       <c r="A273" s="38">
         <v>135</v>
       </c>
@@ -16984,7 +17017,7 @@
       </c>
       <c r="K273" s="22"/>
     </row>
-    <row r="274" spans="1:11" ht="42">
+    <row r="274" spans="1:11" ht="42" hidden="1">
       <c r="A274" s="38">
         <v>137</v>
       </c>
@@ -17054,7 +17087,7 @@
       </c>
       <c r="K275" s="17"/>
     </row>
-    <row r="276" spans="1:11" ht="30">
+    <row r="276" spans="1:11" ht="30" hidden="1">
       <c r="A276" s="38">
         <v>140</v>
       </c>
@@ -17084,7 +17117,7 @@
       </c>
       <c r="K276" s="17"/>
     </row>
-    <row r="277" spans="1:11" ht="45">
+    <row r="277" spans="1:11" ht="45" hidden="1">
       <c r="A277" s="38">
         <v>140</v>
       </c>
@@ -17114,7 +17147,7 @@
       </c>
       <c r="K277" s="17"/>
     </row>
-    <row r="278" spans="1:11" ht="38.25" customHeight="1">
+    <row r="278" spans="1:11" ht="38.25" hidden="1" customHeight="1">
       <c r="A278" s="38">
         <v>140</v>
       </c>
@@ -17181,7 +17214,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="280" spans="1:11" ht="30">
+    <row r="280" spans="1:11" ht="30" hidden="1">
       <c r="A280" s="38">
         <v>141</v>
       </c>
@@ -17218,7 +17251,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="281" spans="1:11" ht="45">
+    <row r="281" spans="1:11" ht="45" hidden="1">
       <c r="A281" s="38">
         <v>141</v>
       </c>
@@ -17255,7 +17288,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="282" spans="1:11" ht="38.25" customHeight="1">
+    <row r="282" spans="1:11" ht="38.25" hidden="1" customHeight="1">
       <c r="A282" s="38">
         <v>141</v>
       </c>
@@ -17330,7 +17363,7 @@
         <v>inoutnetwork</v>
       </c>
     </row>
-    <row r="284" spans="1:11" ht="30">
+    <row r="284" spans="1:11" ht="30" hidden="1">
       <c r="A284" s="38">
         <v>142</v>
       </c>
@@ -17368,7 +17401,7 @@
         <v>inoutnetwork</v>
       </c>
     </row>
-    <row r="285" spans="1:11" ht="38.25" customHeight="1">
+    <row r="285" spans="1:11" ht="38.25" hidden="1" customHeight="1">
       <c r="A285" s="38">
         <v>142</v>
       </c>
@@ -17406,7 +17439,7 @@
         <v>inoutnetwork</v>
       </c>
     </row>
-    <row r="286" spans="1:11" ht="38.25" customHeight="1">
+    <row r="286" spans="1:11" ht="38.25" hidden="1" customHeight="1">
       <c r="A286" s="38">
         <v>142</v>
       </c>
@@ -17444,7 +17477,7 @@
         <v>inoutnetwork</v>
       </c>
     </row>
-    <row r="287" spans="1:11" ht="38.25" customHeight="1">
+    <row r="287" spans="1:11" ht="38.25" hidden="1" customHeight="1">
       <c r="A287" s="38">
         <v>142</v>
       </c>
@@ -17482,7 +17515,7 @@
         <v>inoutnetwork</v>
       </c>
     </row>
-    <row r="288" spans="1:11" ht="38.5" customHeight="1">
+    <row r="288" spans="1:11" ht="38.5" hidden="1" customHeight="1">
       <c r="A288" s="38">
         <v>143</v>
       </c>
@@ -17522,7 +17555,7 @@
         <v>rxorigincode</v>
       </c>
     </row>
-    <row r="289" spans="1:11" ht="38.5" customHeight="1">
+    <row r="289" spans="1:11" ht="38.5" hidden="1" customHeight="1">
       <c r="A289" s="38">
         <v>144</v>
       </c>
@@ -17564,40 +17597,39 @@
     </row>
     <row r="290" spans="1:11" ht="30">
       <c r="A290" s="38">
-        <v>145</v>
-      </c>
-      <c r="B290" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="B290" s="17" t="s">
+        <v>1212</v>
+      </c>
       <c r="C290" s="9" t="s">
-        <v>850</v>
-      </c>
-      <c r="D290" s="61" t="s">
-        <v>851</v>
+        <v>662</v>
+      </c>
+      <c r="D290" s="9" t="s">
+        <v>540</v>
       </c>
       <c r="E290" s="17" t="s">
         <v>1223</v>
       </c>
-      <c r="F290" s="60">
+      <c r="F290" s="50">
         <v>43665</v>
       </c>
       <c r="G290" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$230</f>
+        <f>'EOB Inpatient Institutional'!$B$244</f>
         <v>ExplanationOfBenefit</v>
       </c>
       <c r="H290" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$230</f>
-        <v>diagnosis</v>
-      </c>
-      <c r="I290" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$D$230</f>
-        <v>diagnosis</v>
-      </c>
+        <f>'EOB Inpatient Institutional'!$C$244</f>
+        <v>procedure</v>
+      </c>
+      <c r="I290" s="17"/>
       <c r="J290" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$I$230</f>
-        <v>CodeableConcept</v>
+        <f>'EOB Inpatient Institutional'!$J$244</f>
+        <v>Specific clinical procedure</v>
       </c>
       <c r="K290" s="17"/>
     </row>
-    <row r="291" spans="1:11" ht="30">
+    <row r="291" spans="1:11" ht="30" hidden="1">
       <c r="A291" s="38">
         <v>145</v>
       </c>
@@ -17632,7 +17664,7 @@
       </c>
       <c r="K291" s="17"/>
     </row>
-    <row r="292" spans="1:11" ht="54" customHeight="1">
+    <row r="292" spans="1:11" ht="54" hidden="1" customHeight="1">
       <c r="A292" s="38">
         <v>145</v>
       </c>
@@ -17669,40 +17701,39 @@
     </row>
     <row r="293" spans="1:11" ht="30">
       <c r="A293" s="38">
-        <v>146</v>
-      </c>
-      <c r="B293" s="17"/>
+        <v>27</v>
+      </c>
+      <c r="B293" s="17" t="s">
+        <v>1214</v>
+      </c>
       <c r="C293" s="9" t="s">
-        <v>855</v>
-      </c>
-      <c r="D293" s="61" t="s">
-        <v>856</v>
+        <v>658</v>
+      </c>
+      <c r="D293" s="9" t="s">
+        <v>541</v>
       </c>
       <c r="E293" s="17" t="s">
         <v>1223</v>
       </c>
-      <c r="F293" s="54">
+      <c r="F293" s="50">
         <v>43665</v>
       </c>
       <c r="G293" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$B$230</f>
+        <f>'EOB Inpatient Institutional'!$B$243</f>
         <v>ExplanationOfBenefit</v>
       </c>
       <c r="H293" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$C$230</f>
-        <v>diagnosis</v>
-      </c>
-      <c r="I293" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$D$230</f>
-        <v>diagnosis</v>
-      </c>
+        <f>'EOB Inpatient Institutional'!$C$243</f>
+        <v>procedure</v>
+      </c>
+      <c r="I293" s="17"/>
       <c r="J293" s="17" t="str">
-        <f>'EOB Inpatient Institutional'!$I$230</f>
-        <v>CodeableConcept</v>
+        <f>'EOB Inpatient Institutional'!$J$243</f>
+        <v>When the procedure was performed</v>
       </c>
       <c r="K293" s="17"/>
     </row>
-    <row r="294" spans="1:11" ht="30">
+    <row r="294" spans="1:11" ht="30" hidden="1">
       <c r="A294" s="38">
         <v>147</v>
       </c>
@@ -17737,7 +17768,7 @@
       </c>
       <c r="K294" s="17"/>
     </row>
-    <row r="295" spans="1:11" ht="54" customHeight="1">
+    <row r="295" spans="1:11" ht="54" hidden="1" customHeight="1">
       <c r="A295" s="38">
         <v>147</v>
       </c>
@@ -17812,7 +17843,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="297" spans="1:11" ht="132" customHeight="1">
+    <row r="297" spans="1:11" ht="132" hidden="1" customHeight="1">
       <c r="A297" s="38">
         <v>148</v>
       </c>
@@ -17852,7 +17883,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="298" spans="1:11" ht="121" customHeight="1">
+    <row r="298" spans="1:11" ht="121" hidden="1" customHeight="1">
       <c r="A298" s="38">
         <v>148</v>
       </c>
@@ -17892,7 +17923,7 @@
         <v>adjudicationamounttype</v>
       </c>
     </row>
-    <row r="299" spans="1:11" ht="162" customHeight="1">
+    <row r="299" spans="1:11" ht="162" hidden="1" customHeight="1">
       <c r="A299" s="38">
         <v>148</v>
       </c>
@@ -17970,7 +18001,7 @@
         <v>allowedunits</v>
       </c>
     </row>
-    <row r="301" spans="1:11" ht="56">
+    <row r="301" spans="1:11" ht="56" hidden="1">
       <c r="A301" s="38">
         <v>149</v>
       </c>
@@ -18008,7 +18039,7 @@
         <v>allowedunits</v>
       </c>
     </row>
-    <row r="302" spans="1:11" ht="56">
+    <row r="302" spans="1:11" ht="56" hidden="1">
       <c r="A302" s="38">
         <v>149</v>
       </c>
@@ -18046,7 +18077,7 @@
         <v>allowedunits</v>
       </c>
     </row>
-    <row r="303" spans="1:11" ht="30">
+    <row r="303" spans="1:11" ht="30" hidden="1">
       <c r="A303" s="38">
         <v>150</v>
       </c>
@@ -18081,7 +18112,7 @@
       </c>
       <c r="K303" s="22"/>
     </row>
-    <row r="304" spans="1:11" ht="34">
+    <row r="304" spans="1:11" ht="34" hidden="1">
       <c r="A304" s="38">
         <v>151</v>
       </c>
@@ -18118,7 +18149,7 @@
       </c>
       <c r="K304" s="22"/>
     </row>
-    <row r="305" spans="1:11" ht="38.25" customHeight="1">
+    <row r="305" spans="1:11" ht="38.25" hidden="1" customHeight="1">
       <c r="A305" s="38">
         <v>152</v>
       </c>
@@ -18143,7 +18174,7 @@
       <c r="J305" s="66"/>
       <c r="K305" s="66"/>
     </row>
-    <row r="306" spans="1:11" ht="30">
+    <row r="306" spans="1:11" ht="30" hidden="1">
       <c r="A306" s="38">
         <v>153</v>
       </c>
@@ -18175,7 +18206,7 @@
       </c>
       <c r="K306" s="22"/>
     </row>
-    <row r="307" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="307" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A307" s="38">
         <v>154</v>
       </c>
@@ -18210,7 +18241,7 @@
       </c>
       <c r="K307" s="15"/>
     </row>
-    <row r="308" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="308" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A308" s="38">
         <v>155</v>
       </c>
@@ -18245,7 +18276,7 @@
       </c>
       <c r="K308" s="15"/>
     </row>
-    <row r="309" spans="1:11" ht="30">
+    <row r="309" spans="1:11" ht="30" hidden="1">
       <c r="A309" s="38">
         <v>158</v>
       </c>
@@ -18308,7 +18339,7 @@
         <v>Metadata about the resource</v>
       </c>
     </row>
-    <row r="311" spans="1:11" ht="30">
+    <row r="311" spans="1:11" ht="30" hidden="1">
       <c r="A311" s="39">
         <v>163</v>
       </c>
@@ -18339,7 +18370,7 @@
         <v>Metadata about the resource</v>
       </c>
     </row>
-    <row r="312" spans="1:11" ht="45">
+    <row r="312" spans="1:11" ht="45" hidden="1">
       <c r="A312" s="39">
         <v>163</v>
       </c>
@@ -18370,7 +18401,7 @@
         <v>Metadata about the resource</v>
       </c>
     </row>
-    <row r="313" spans="1:11" ht="30">
+    <row r="313" spans="1:11" ht="30" hidden="1">
       <c r="A313" s="39">
         <v>163</v>
       </c>
@@ -18401,7 +18432,7 @@
         <v>Metadata about the resource</v>
       </c>
     </row>
-    <row r="314" spans="1:11" ht="45">
+    <row r="314" spans="1:11" ht="45" hidden="1">
       <c r="A314" s="38">
         <v>163</v>
       </c>
@@ -18433,7 +18464,7 @@
       </c>
       <c r="K314" s="23"/>
     </row>
-    <row r="315" spans="1:11" ht="30">
+    <row r="315" spans="1:11" ht="30" hidden="1">
       <c r="A315" s="38">
         <v>163</v>
       </c>
@@ -18465,7 +18496,7 @@
       </c>
       <c r="K315" s="23"/>
     </row>
-    <row r="316" spans="1:11" ht="30">
+    <row r="316" spans="1:11" ht="30" hidden="1">
       <c r="A316" s="38">
         <v>163</v>
       </c>
@@ -18497,7 +18528,7 @@
       </c>
       <c r="K316" s="23"/>
     </row>
-    <row r="317" spans="1:11" s="8" customFormat="1">
+    <row r="317" spans="1:11" s="8" customFormat="1" hidden="1">
       <c r="A317" s="38">
         <v>164</v>
       </c>
@@ -18547,7 +18578,7 @@
       </c>
       <c r="K318" s="23"/>
     </row>
-    <row r="319" spans="1:11" ht="30">
+    <row r="319" spans="1:11" ht="30" hidden="1">
       <c r="A319" s="39">
         <v>165</v>
       </c>
@@ -18582,7 +18613,7 @@
       </c>
       <c r="K319" s="23"/>
     </row>
-    <row r="320" spans="1:11" ht="45">
+    <row r="320" spans="1:11" ht="45" hidden="1">
       <c r="A320" s="39">
         <v>165</v>
       </c>
@@ -18617,7 +18648,7 @@
       </c>
       <c r="K320" s="23"/>
     </row>
-    <row r="321" spans="1:11" ht="30">
+    <row r="321" spans="1:11" ht="30" hidden="1">
       <c r="A321" s="39">
         <v>165</v>
       </c>
@@ -18690,7 +18721,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="323" spans="1:11" ht="30">
+    <row r="323" spans="1:11" ht="30" hidden="1">
       <c r="A323" s="38">
         <v>166</v>
       </c>
@@ -18763,7 +18794,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="325" spans="1:11" ht="30">
+    <row r="325" spans="1:11" ht="30" hidden="1">
       <c r="A325" s="38">
         <v>167</v>
       </c>
@@ -18798,7 +18829,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="326" spans="1:11" ht="45">
+    <row r="326" spans="1:11" ht="45" hidden="1">
       <c r="A326" s="38">
         <v>167</v>
       </c>
@@ -18833,7 +18864,7 @@
         <v>Reference(Practitioner | Organization)</v>
       </c>
     </row>
-    <row r="327" spans="1:11" ht="30">
+    <row r="327" spans="1:11" ht="30" hidden="1">
       <c r="A327" s="38">
         <v>167</v>
       </c>
@@ -18868,7 +18899,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="328" spans="1:11" ht="71">
+    <row r="328" spans="1:11" ht="71" hidden="1">
       <c r="A328" s="38">
         <v>168</v>
       </c>
@@ -18941,7 +18972,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="330" spans="1:11" ht="30">
+    <row r="330" spans="1:11" ht="30" hidden="1">
       <c r="A330" s="38">
         <v>169</v>
       </c>
@@ -18979,7 +19010,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="331" spans="1:11" ht="45">
+    <row r="331" spans="1:11" ht="45" hidden="1">
       <c r="A331" s="38">
         <v>169</v>
       </c>
@@ -19014,7 +19045,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="332" spans="1:11" ht="30">
+    <row r="332" spans="1:11" ht="30" hidden="1">
       <c r="A332" s="38">
         <v>169</v>
       </c>
@@ -19052,7 +19083,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="333" spans="1:11" ht="71">
+    <row r="333" spans="1:11" ht="71" hidden="1">
       <c r="A333" s="38">
         <v>170</v>
       </c>
@@ -19128,7 +19159,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="335" spans="1:11" ht="30">
+    <row r="335" spans="1:11" ht="30" hidden="1">
       <c r="A335" s="38">
         <v>171</v>
       </c>
@@ -19166,7 +19197,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="336" spans="1:11" ht="45">
+    <row r="336" spans="1:11" ht="45" hidden="1">
       <c r="A336" s="38">
         <v>171</v>
       </c>
@@ -19201,7 +19232,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="337" spans="1:11" ht="30">
+    <row r="337" spans="1:11" ht="30" hidden="1">
       <c r="A337" s="38">
         <v>172</v>
       </c>
@@ -19277,7 +19308,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="339" spans="1:11" ht="52.5" customHeight="1">
+    <row r="339" spans="1:11" ht="52.5" hidden="1" customHeight="1">
       <c r="A339" s="38">
         <v>173</v>
       </c>
@@ -19353,7 +19384,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="341" spans="1:11" ht="30">
+    <row r="341" spans="1:11" ht="30" hidden="1">
       <c r="A341" s="38">
         <v>174</v>
       </c>
@@ -19461,7 +19492,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="344" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="344" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A344" s="39">
         <v>175</v>
       </c>
@@ -19496,7 +19527,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="345" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="345" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A345" s="39">
         <v>175</v>
       </c>
@@ -19531,7 +19562,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="346" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="346" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A346" s="39">
         <v>175</v>
       </c>
@@ -19566,7 +19597,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="347" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="347" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A347" s="39">
         <v>175</v>
       </c>
@@ -19601,7 +19632,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="348" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="348" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A348" s="39">
         <v>175</v>
       </c>
@@ -19636,7 +19667,7 @@
         <v>Reference(Organization)</v>
       </c>
     </row>
-    <row r="349" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="349" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A349" s="39">
         <v>175</v>
       </c>
@@ -19671,7 +19702,7 @@
         <v>Reference(Coverage)</v>
       </c>
     </row>
-    <row r="350" spans="1:11" ht="80" customHeight="1">
+    <row r="350" spans="1:11" ht="80" hidden="1" customHeight="1">
       <c r="A350" s="38">
         <v>176</v>
       </c>
@@ -19747,7 +19778,7 @@
       </c>
       <c r="K351" s="17"/>
     </row>
-    <row r="352" spans="1:11" s="8" customFormat="1" ht="73.5" customHeight="1">
+    <row r="352" spans="1:11" s="8" customFormat="1" ht="73.5" hidden="1" customHeight="1">
       <c r="A352" s="39">
         <v>177</v>
       </c>
@@ -19785,7 +19816,7 @@
       </c>
       <c r="K352" s="17"/>
     </row>
-    <row r="353" spans="1:11" s="8" customFormat="1" ht="73.5" customHeight="1">
+    <row r="353" spans="1:11" s="8" customFormat="1" ht="73.5" hidden="1" customHeight="1">
       <c r="A353" s="39">
         <v>177</v>
       </c>
@@ -19861,7 +19892,7 @@
       </c>
       <c r="K354" s="17"/>
     </row>
-    <row r="355" spans="1:11" s="8" customFormat="1" ht="56">
+    <row r="355" spans="1:11" s="8" customFormat="1" ht="56" hidden="1">
       <c r="A355" s="38">
         <v>178</v>
       </c>
@@ -19899,7 +19930,7 @@
       </c>
       <c r="K355" s="17"/>
     </row>
-    <row r="356" spans="1:11" s="8" customFormat="1" ht="45">
+    <row r="356" spans="1:11" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A356" s="38">
         <v>178</v>
       </c>
@@ -19972,7 +20003,7 @@
       </c>
       <c r="K357" s="17"/>
     </row>
-    <row r="358" spans="1:11" s="8" customFormat="1" ht="30">
+    <row r="358" spans="1:11" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A358" s="38">
         <v>179</v>
       </c>
@@ -20007,7 +20038,7 @@
       </c>
       <c r="K358" s="17"/>
     </row>
-    <row r="359" spans="1:11" ht="45">
+    <row r="359" spans="1:11" ht="45" hidden="1">
       <c r="A359" s="38">
         <v>179</v>
       </c>
@@ -20042,7 +20073,7 @@
       </c>
       <c r="K359" s="17"/>
     </row>
-    <row r="360" spans="1:11">
+    <row r="360" spans="1:11" hidden="1">
       <c r="A360" s="38">
         <v>179</v>
       </c>
@@ -20077,7 +20108,7 @@
       </c>
       <c r="K360" s="17"/>
     </row>
-    <row r="361" spans="1:11" ht="45">
+    <row r="361" spans="1:11" ht="45" hidden="1">
       <c r="A361" s="38">
         <v>180</v>
       </c>
@@ -20144,7 +20175,7 @@
       </c>
       <c r="K362" s="17"/>
     </row>
-    <row r="363" spans="1:11" ht="45">
+    <row r="363" spans="1:11" ht="45" hidden="1">
       <c r="A363" s="38">
         <v>181</v>
       </c>
@@ -20179,7 +20210,7 @@
       </c>
       <c r="K363" s="17"/>
     </row>
-    <row r="364" spans="1:11" ht="45">
+    <row r="364" spans="1:11" ht="45" hidden="1">
       <c r="A364" s="38">
         <v>181</v>
       </c>
@@ -20214,7 +20245,7 @@
       </c>
       <c r="K364" s="17"/>
     </row>
-    <row r="365" spans="1:11" ht="45">
+    <row r="365" spans="1:11" ht="45" hidden="1">
       <c r="A365" s="38">
         <v>181</v>
       </c>
@@ -20287,7 +20318,7 @@
         <v>Reference(Practitioner)</v>
       </c>
     </row>
-    <row r="367" spans="1:11" ht="30">
+    <row r="367" spans="1:11" ht="30" hidden="1">
       <c r="A367" s="38">
         <v>182</v>
       </c>
@@ -20326,7 +20357,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K367" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:K367" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="EOB Inpatient Institutional"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A124:K293">
+      <sortCondition ref="H1:H367"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F109">
     <sortCondition ref="A2:A109"/>
   </sortState>
@@ -20339,9 +20379,6 @@
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="G269" formula="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -20354,7 +20391,7 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L374" sqref="L374"/>
       <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
@@ -26950,10 +26987,10 @@
   </sheetPr>
   <dimension ref="A1:CI475"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L374" sqref="L374"/>
-      <selection pane="bottomLeft" activeCell="L147" sqref="L147"/>
+      <selection pane="bottomLeft" activeCell="A198" sqref="A198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -38663,10 +38700,10 @@
   </sheetPr>
   <dimension ref="A1:R424"/>
   <sheetViews>
-    <sheetView zoomScale="67" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H5" sqref="H5"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A247" sqref="A247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>